<commit_message>
AtualizaSensores ajustado | erro na planilha
</commit_message>
<xml_diff>
--- a/BankServiceRepport.xlsx
+++ b/BankServiceRepport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>Pagador</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>MobilityCompany</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -70,7 +76,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,6 +94,90 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>45262.712759699076</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>45262.713720023145</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>45262.71517917824</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>45262.71607657408</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>45262.71751649305</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>45262.718644444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planilhas OK | Falta estatisicas
</commit_message>
<xml_diff>
--- a/BankServiceRepport.xlsx
+++ b/BankServiceRepport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Pagador</t>
   </si>
@@ -76,7 +76,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -107,7 +107,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>45262.712759699076</v>
+        <v>45262.742241851854</v>
       </c>
     </row>
     <row r="3">
@@ -121,7 +121,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>45262.713720023145</v>
+        <v>45262.743162743056</v>
       </c>
     </row>
     <row r="4">
@@ -135,7 +135,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>45262.71517917824</v>
+        <v>45262.74417859954</v>
       </c>
     </row>
     <row r="5">
@@ -149,35 +149,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>45262.71607657408</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>45262.71751649305</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>45262.718644444445</v>
+        <v>45262.744987592596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planilha OK | Faltam graficos
</commit_message>
<xml_diff>
--- a/BankServiceRepport.xlsx
+++ b/BankServiceRepport.xlsx
@@ -107,7 +107,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>45263.09483810185</v>
+        <v>45263.51879659722</v>
       </c>
     </row>
     <row r="3">
@@ -121,7 +121,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>45263.09532380787</v>
+        <v>45263.519293310186</v>
       </c>
     </row>
     <row r="4">
@@ -135,7 +135,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>45263.0958902662</v>
+        <v>45263.51985621528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>